<commit_message>
Created a new folder for the ChessBoard.fxml file that has the chessboard Visuals that I hope to connect with the rest of my code. The credits links for the chess icons are in the dev blog
</commit_message>
<xml_diff>
--- a/Blog_Hours_Sheet.xlsx
+++ b/Blog_Hours_Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Computer_Science\CS25320\chess-personal-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\callu\IdeaProjects\Chess-Personal-Project-GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2CB57F-E357-4D1B-93EE-EFAAEF9E7A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AAEF84-4698-4580-914A-15186933508F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12120" xr2:uid="{62F9DC62-69F3-4F1D-8CD0-BA0478732F4B}"/>
+    <workbookView xWindow="5760" yWindow="120" windowWidth="17280" windowHeight="8928" xr2:uid="{62F9DC62-69F3-4F1D-8CD0-BA0478732F4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,11 +515,13 @@
       <c r="E2" s="2">
         <v>2.5</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="4">
         <f>SUM(A2:G2)</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>